<commit_message>
#105358 Update decimal places on columns
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74273BE0-297D-41D2-8020-2536CE5AB6A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C78FDFF-3A4A-43A4-9696-5C7F9DA101CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -205,8 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
@@ -327,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -511,9 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -526,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -864,40 +857,40 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.46484375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" style="21" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="12.86328125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="15.86328125" style="34" customWidth="1"/>
-    <col min="10" max="10" width="13.19921875" style="34" customWidth="1"/>
-    <col min="11" max="11" width="12.86328125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="12.86328125" style="34" customWidth="1"/>
-    <col min="13" max="13" width="15.86328125" style="34" customWidth="1"/>
-    <col min="14" max="14" width="14.73046875" style="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.9296875" style="34" customWidth="1"/>
-    <col min="16" max="16" width="12.86328125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="12.86328125" style="34" customWidth="1"/>
-    <col min="18" max="18" width="15.86328125" style="34" customWidth="1"/>
-    <col min="19" max="19" width="17.53125" style="34" customWidth="1"/>
-    <col min="20" max="20" width="12.86328125" style="34" customWidth="1"/>
-    <col min="21" max="21" width="12.86328125" style="21" customWidth="1"/>
-    <col min="22" max="22" width="12.86328125" style="34" customWidth="1"/>
-    <col min="23" max="23" width="15.86328125" style="34" customWidth="1"/>
-    <col min="24" max="24" width="16.86328125" style="34" customWidth="1"/>
-    <col min="25" max="25" width="8.86328125" style="34"/>
-    <col min="26" max="16384" width="8.86328125" style="2"/>
+    <col min="7" max="7" width="12.88671875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="34" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" style="34" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="21" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="34" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" style="34" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" style="34" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" style="21" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" style="34" customWidth="1"/>
+    <col min="18" max="18" width="15.88671875" style="34" customWidth="1"/>
+    <col min="19" max="19" width="17.5546875" style="34" customWidth="1"/>
+    <col min="20" max="20" width="12.88671875" style="34" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" style="21" customWidth="1"/>
+    <col min="22" max="22" width="12.88671875" style="34" customWidth="1"/>
+    <col min="23" max="23" width="15.88671875" style="34" customWidth="1"/>
+    <col min="24" max="24" width="16.88671875" style="34" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" style="34"/>
+    <col min="26" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -915,7 +908,7 @@
       <c r="V1" s="55"/>
       <c r="X1" s="27"/>
     </row>
-    <row r="2" spans="1:25" ht="23.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -949,7 +942,7 @@
       <c r="W2" s="57"/>
       <c r="X2" s="35"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -967,7 +960,7 @@
       <c r="U3" s="59"/>
       <c r="X3" s="27"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="D4" s="14"/>
@@ -981,7 +974,7 @@
       <c r="U4" s="59"/>
       <c r="X4" s="27"/>
     </row>
-    <row r="5" spans="1:25" s="43" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" s="43" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -1055,7 +1048,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D6" s="20"/>
       <c r="E6" s="22"/>
       <c r="F6" s="29"/>
@@ -1079,7 +1072,7 @@
       <c r="X6" s="29"/>
       <c r="Y6" s="43"/>
     </row>
-    <row r="7" spans="1:25" s="44" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1108,7 +1101,7 @@
       <c r="X7" s="30"/>
       <c r="Y7" s="60"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1111,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="31"/>
@@ -1149,204 +1142,204 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="71">
+      <c r="I9" s="68"/>
+      <c r="J9" s="69">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="70"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="71">
+      <c r="M9" s="68"/>
+      <c r="N9" s="69">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="70"/>
+      <c r="P9" s="67"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="72"/>
-      <c r="S9" s="71">
+      <c r="R9" s="68"/>
+      <c r="S9" s="69">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="70"/>
+      <c r="U9" s="67"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="72"/>
-      <c r="X9" s="71">
+      <c r="W9" s="68"/>
+      <c r="X9" s="69">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="68"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="70"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="71"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="69"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="70"/>
+      <c r="P10" s="67"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="71"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="69"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="70"/>
+      <c r="U10" s="67"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="72"/>
-      <c r="X10" s="71"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="73"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="71">
+      <c r="I11" s="68"/>
+      <c r="J11" s="69">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="70"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="71">
+      <c r="M11" s="68"/>
+      <c r="N11" s="69">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="70"/>
+      <c r="P11" s="67"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="72"/>
-      <c r="S11" s="71">
+      <c r="R11" s="68"/>
+      <c r="S11" s="69">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="70"/>
+      <c r="U11" s="67"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="71">
+      <c r="W11" s="68"/>
+      <c r="X11" s="69">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="68"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="70"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="71"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="70"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="71"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="69"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="70"/>
+      <c r="U12" s="67"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="72"/>
-      <c r="X12" s="71"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="W12" s="68"/>
+      <c r="X12" s="69"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="73"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="71">
+      <c r="I13" s="68"/>
+      <c r="J13" s="69">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="70"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="71">
+      <c r="M13" s="68"/>
+      <c r="N13" s="69">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="70"/>
+      <c r="P13" s="67"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="71">
+      <c r="R13" s="68"/>
+      <c r="S13" s="69">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="70"/>
+      <c r="U13" s="67"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="72"/>
-      <c r="X13" s="71">
+      <c r="W13" s="68"/>
+      <c r="X13" s="69">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="68"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1354,27 +1347,27 @@
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="71"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="71"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="69"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="70"/>
-      <c r="V14" s="63"/>
-      <c r="W14" s="72"/>
-      <c r="X14" s="71"/>
-    </row>
-    <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="U14" s="67"/>
+      <c r="V14" s="61"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="69"/>
+    </row>
+    <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1378,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="25"/>
       <c r="F15" s="37"/>
-      <c r="G15" s="64"/>
+      <c r="G15" s="63"/>
       <c r="H15" s="26">
         <f>SUM(H8:H14)</f>
         <v>0</v>
@@ -1398,7 +1391,7 @@
         <f>SUM(J8:J14)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="64"/>
+      <c r="K15" s="63"/>
       <c r="L15" s="26">
         <f>SUM(L8:L14)</f>
         <v>0</v>
@@ -1426,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="54"/>
-      <c r="U15" s="64"/>
+      <c r="U15" s="63"/>
       <c r="V15" s="26">
         <f>SUM(V8:V14)</f>
         <v>0</v>
@@ -1439,9 +1432,9 @@
         <f>SUM(X8:X14)</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="65"/>
-    </row>
-    <row r="16" spans="1:25" s="50" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y15" s="64"/>
+    </row>
+    <row r="16" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
@@ -1482,9 +1475,9 @@
         <v>0</v>
       </c>
       <c r="X16" s="38"/>
-      <c r="Y16" s="66"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="Y16" s="65"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D17" s="14"/>
       <c r="F17" s="36"/>
       <c r="I17" s="21"/>
@@ -1496,7 +1489,7 @@
       <c r="W17" s="21"/>
       <c r="X17" s="36"/>
     </row>
-    <row r="18" spans="1:25" s="44" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -1525,7 +1518,7 @@
       <c r="X18" s="30"/>
       <c r="Y18" s="60"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1528,7 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="41"/>
@@ -1566,204 +1559,204 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="73"/>
+      <c r="D20" s="70"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="70"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="71">
+      <c r="I20" s="68"/>
+      <c r="J20" s="69">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="70"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="71">
+      <c r="M20" s="68"/>
+      <c r="N20" s="69">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="70"/>
+      <c r="P20" s="67"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="71">
+      <c r="R20" s="68"/>
+      <c r="S20" s="69">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="70"/>
+      <c r="U20" s="67"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="72"/>
-      <c r="X20" s="71">
+      <c r="W20" s="68"/>
+      <c r="X20" s="69">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="68"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="70" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="70"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="70"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="67"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="71"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="70"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="72"/>
-      <c r="S21" s="71"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="69"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="70"/>
+      <c r="U21" s="67"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="72"/>
-      <c r="X21" s="71"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="W21" s="68"/>
+      <c r="X21" s="69"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="73"/>
+      <c r="D22" s="70"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="70"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="71">
+      <c r="I22" s="68"/>
+      <c r="J22" s="69">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="70"/>
+      <c r="K22" s="67"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="71">
+      <c r="M22" s="68"/>
+      <c r="N22" s="69">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="70"/>
+      <c r="P22" s="67"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="72"/>
-      <c r="S22" s="71">
+      <c r="R22" s="68"/>
+      <c r="S22" s="69">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="70"/>
+      <c r="U22" s="67"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="71">
+      <c r="W22" s="68"/>
+      <c r="X22" s="69">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="68"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="70"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="70"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="67"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="71"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="69"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="70"/>
+      <c r="P23" s="67"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="71"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="70"/>
+      <c r="U23" s="67"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="72"/>
-      <c r="X23" s="71"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="W23" s="68"/>
+      <c r="X23" s="69"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="73"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="70"/>
+      <c r="G24" s="67"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="71">
+      <c r="I24" s="68"/>
+      <c r="J24" s="69">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="70"/>
+      <c r="K24" s="67"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="71">
+      <c r="M24" s="68"/>
+      <c r="N24" s="69">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="70"/>
+      <c r="P24" s="67"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="72"/>
-      <c r="S24" s="71">
+      <c r="R24" s="68"/>
+      <c r="S24" s="69">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="70"/>
+      <c r="U24" s="67"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="72"/>
-      <c r="X24" s="71">
+      <c r="W24" s="68"/>
+      <c r="X24" s="69">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="68"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1772,26 +1765,26 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="70"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="70"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="67"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="71"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="69"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="70"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="72"/>
-      <c r="S25" s="71"/>
+      <c r="R25" s="68"/>
+      <c r="S25" s="69"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="70"/>
+      <c r="U25" s="67"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="72"/>
-      <c r="X25" s="71"/>
-    </row>
-    <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="W25" s="68"/>
+      <c r="X25" s="69"/>
+    </row>
+    <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
         <v>13</v>
       </c>
@@ -1802,7 +1795,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="26"/>
       <c r="F26" s="42"/>
-      <c r="G26" s="64"/>
+      <c r="G26" s="63"/>
       <c r="H26" s="26">
         <f>SUM(H19:H25)</f>
         <v>0</v>
@@ -1815,7 +1808,7 @@
         <f>SUM(J19:J25)</f>
         <v>0</v>
       </c>
-      <c r="K26" s="64"/>
+      <c r="K26" s="63"/>
       <c r="L26" s="26">
         <f>SUM(L19:L25)</f>
         <v>0</v>
@@ -1843,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="T26" s="54"/>
-      <c r="U26" s="64"/>
+      <c r="U26" s="63"/>
       <c r="V26" s="26">
         <f>SUM(V19:V25)</f>
         <v>0</v>
@@ -1856,9 +1849,9 @@
         <f>SUM(X19:X25)</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="65"/>
-    </row>
-    <row r="27" spans="1:25" s="50" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y26" s="64"/>
+    </row>
+    <row r="27" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
@@ -1899,33 +1892,33 @@
         <v>0</v>
       </c>
       <c r="X27" s="38"/>
-      <c r="Y27" s="66"/>
-    </row>
-    <row r="28" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="Y27" s="65"/>
+    </row>
+    <row r="28" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D28" s="47"/>
       <c r="E28" s="48"/>
       <c r="F28" s="51"/>
       <c r="G28" s="48"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
       <c r="J28" s="51"/>
       <c r="K28" s="48"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
       <c r="N28" s="51"/>
-      <c r="O28" s="65"/>
+      <c r="O28" s="64"/>
       <c r="P28" s="48"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="65"/>
+      <c r="Q28" s="64"/>
+      <c r="R28" s="64"/>
       <c r="S28" s="51"/>
-      <c r="T28" s="65"/>
+      <c r="T28" s="64"/>
       <c r="U28" s="48"/>
-      <c r="V28" s="65"/>
-      <c r="W28" s="65"/>
+      <c r="V28" s="64"/>
+      <c r="W28" s="64"/>
       <c r="X28" s="51"/>
-      <c r="Y28" s="65"/>
-    </row>
-    <row r="29" spans="1:25" s="44" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y28" s="64"/>
+    </row>
+    <row r="29" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>45</v>
       </c>
@@ -1954,7 +1947,7 @@
       <c r="X29" s="30"/>
       <c r="Y29" s="60"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -1964,7 +1957,7 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="73" t="s">
+      <c r="D30" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="24"/>
@@ -1988,7 +1981,7 @@
       <c r="W30" s="24"/>
       <c r="X30" s="39"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -1998,7 +1991,7 @@
       <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="73"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2020,7 +2013,7 @@
       <c r="W31" s="24"/>
       <c r="X31" s="39"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +2047,7 @@
       <c r="W32" s="24"/>
       <c r="X32" s="39"/>
     </row>
-    <row r="33" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="32" t="s">
         <v>22</v>
       </c>
@@ -2075,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="37"/>
-      <c r="K33" s="64"/>
+      <c r="K33" s="63"/>
       <c r="L33" s="18">
         <f>SUM(L27:L32)</f>
         <v>0</v>
@@ -2086,7 +2079,7 @@
       </c>
       <c r="N33" s="37"/>
       <c r="O33" s="54"/>
-      <c r="P33" s="64"/>
+      <c r="P33" s="63"/>
       <c r="Q33" s="18">
         <f>SUM(Q27:Q32)</f>
         <v>0</v>
@@ -2097,7 +2090,7 @@
       </c>
       <c r="S33" s="37"/>
       <c r="T33" s="54"/>
-      <c r="U33" s="64"/>
+      <c r="U33" s="63"/>
       <c r="V33" s="18">
         <f>SUM(V27:V32)</f>
         <v>0</v>
@@ -2107,9 +2100,9 @@
         <v>0</v>
       </c>
       <c r="X33" s="37"/>
-      <c r="Y33" s="65"/>
-    </row>
-    <row r="34" spans="1:25" s="50" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y33" s="64"/>
+    </row>
+    <row r="34" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>22</v>
       </c>
@@ -2150,35 +2143,35 @@
         <v>0</v>
       </c>
       <c r="X34" s="38"/>
-      <c r="Y34" s="66"/>
-    </row>
-    <row r="35" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="Y34" s="65"/>
+    </row>
+    <row r="35" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="45"/>
       <c r="B35" s="46"/>
       <c r="D35" s="47"/>
       <c r="E35" s="48"/>
       <c r="F35" s="52"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="67"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="66"/>
       <c r="J35" s="49"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="65"/>
-      <c r="M35" s="67"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="66"/>
       <c r="N35" s="49"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="65"/>
-      <c r="R35" s="67"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="64"/>
+      <c r="R35" s="66"/>
       <c r="S35" s="49"/>
-      <c r="T35" s="65"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="65"/>
-      <c r="W35" s="67"/>
+      <c r="T35" s="64"/>
+      <c r="U35" s="66"/>
+      <c r="V35" s="64"/>
+      <c r="W35" s="66"/>
       <c r="X35" s="49"/>
-      <c r="Y35" s="65"/>
-    </row>
-    <row r="36" spans="1:25" s="44" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y35" s="64"/>
+    </row>
+    <row r="36" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>46</v>
       </c>
@@ -2207,7 +2200,7 @@
       <c r="X36" s="30"/>
       <c r="Y36" s="60"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
@@ -2217,7 +2210,7 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="73" t="s">
+      <c r="D37" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="24"/>
@@ -2241,7 +2234,7 @@
       <c r="W37" s="62"/>
       <c r="X37" s="39"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
@@ -2251,7 +2244,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="73"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2273,7 +2266,7 @@
       <c r="W38" s="62"/>
       <c r="X38" s="39"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
@@ -2307,7 +2300,7 @@
       <c r="W39" s="62"/>
       <c r="X39" s="39"/>
     </row>
-    <row r="40" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="s">
         <v>21</v>
       </c>
@@ -2320,7 +2313,7 @@
       <c r="F40" s="37">
         <v>0</v>
       </c>
-      <c r="G40" s="64"/>
+      <c r="G40" s="63"/>
       <c r="H40" s="26">
         <f>SUM(H37:H39)</f>
         <v>0</v>
@@ -2330,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="37"/>
-      <c r="K40" s="64"/>
+      <c r="K40" s="63"/>
       <c r="L40" s="18">
         <f>SUM(L34:L39)</f>
         <v>0</v>
@@ -2341,7 +2334,7 @@
       </c>
       <c r="N40" s="37"/>
       <c r="O40" s="54"/>
-      <c r="P40" s="64"/>
+      <c r="P40" s="63"/>
       <c r="Q40" s="18">
         <f>SUM(Q34:Q39)</f>
         <v>0</v>
@@ -2355,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="T40" s="54"/>
-      <c r="U40" s="64"/>
+      <c r="U40" s="63"/>
       <c r="V40" s="18">
         <f>SUM(V34:V39)</f>
         <v>0</v>
@@ -2365,9 +2358,9 @@
         <v>0</v>
       </c>
       <c r="X40" s="37"/>
-      <c r="Y40" s="65"/>
-    </row>
-    <row r="41" spans="1:25" s="50" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
+      <c r="Y40" s="64"/>
+    </row>
+    <row r="41" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>21</v>
       </c>
@@ -2411,87 +2404,13 @@
         <v>0</v>
       </c>
       <c r="X41" s="38"/>
-      <c r="Y41" s="66"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="Y41" s="65"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43"/>
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2507,6 +2426,80 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#105413 Updating sheet name
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C78FDFF-3A4A-43A4-9696-5C7F9DA101CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37413A0-4C99-4462-AAA8-238AAFAC15D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BetaCrossYearIndicativePayments" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -519,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1111,7 +1111,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="72" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="31"/>
@@ -1146,41 +1146,41 @@
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="67" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="67"/>
+      <c r="D9" s="72"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="69">
+      <c r="I9" s="71"/>
+      <c r="J9" s="70">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="67"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="69">
+      <c r="M9" s="71"/>
+      <c r="N9" s="70">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="67"/>
+      <c r="P9" s="69"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="69">
+      <c r="R9" s="71"/>
+      <c r="S9" s="70">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="67"/>
+      <c r="U9" s="69"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="68"/>
-      <c r="X9" s="69">
+      <c r="W9" s="71"/>
+      <c r="X9" s="70">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
@@ -1189,72 +1189,72 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="67"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="69"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="67"/>
+      <c r="P10" s="69"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="69"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="70"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="67"/>
+      <c r="U10" s="69"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="68"/>
-      <c r="X10" s="69"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="70"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="67" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="67"/>
+      <c r="D11" s="72"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69">
+      <c r="I11" s="71"/>
+      <c r="J11" s="70">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="69">
+      <c r="M11" s="71"/>
+      <c r="N11" s="70">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="67"/>
+      <c r="P11" s="69"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="69">
+      <c r="R11" s="71"/>
+      <c r="S11" s="70">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="67"/>
+      <c r="U11" s="69"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="69">
+      <c r="W11" s="71"/>
+      <c r="X11" s="70">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
@@ -1263,74 +1263,74 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="71"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="67"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="69"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="69"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="70"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="67"/>
+      <c r="P12" s="69"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="70"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="67"/>
+      <c r="U12" s="69"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="69"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="70"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="67" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="70"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="69">
+      <c r="I13" s="71"/>
+      <c r="J13" s="70">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="67"/>
+      <c r="K13" s="69"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="69">
+      <c r="M13" s="71"/>
+      <c r="N13" s="70">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="67"/>
+      <c r="P13" s="69"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69">
+      <c r="R13" s="71"/>
+      <c r="S13" s="70">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="67"/>
+      <c r="U13" s="69"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="68"/>
-      <c r="X13" s="69">
+      <c r="W13" s="71"/>
+      <c r="X13" s="70">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1347,25 +1347,25 @@
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="67"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="69"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="69"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="70"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="67"/>
+      <c r="P14" s="69"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="70"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="67"/>
+      <c r="U14" s="69"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="69"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="70"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -1528,7 +1528,7 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="72" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="41"/>
@@ -1563,41 +1563,41 @@
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="67" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="70"/>
+      <c r="D20" s="72"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="67"/>
+      <c r="G20" s="69"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="69">
+      <c r="I20" s="71"/>
+      <c r="J20" s="70">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="67"/>
+      <c r="K20" s="69"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="69">
+      <c r="M20" s="71"/>
+      <c r="N20" s="70">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="67"/>
+      <c r="P20" s="69"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="69">
+      <c r="R20" s="71"/>
+      <c r="S20" s="70">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="67"/>
+      <c r="U20" s="69"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="68"/>
-      <c r="X20" s="69">
+      <c r="W20" s="71"/>
+      <c r="X20" s="70">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
@@ -1606,72 +1606,72 @@
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D21" s="72" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="67"/>
+      <c r="G21" s="69"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="67"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="69"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="69"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="70"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="67"/>
+      <c r="P21" s="69"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="69"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="70"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="67"/>
+      <c r="U21" s="69"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="68"/>
-      <c r="X21" s="69"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="70"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="67" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="70"/>
+      <c r="D22" s="72"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="67"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="69">
+      <c r="I22" s="71"/>
+      <c r="J22" s="70">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="67"/>
+      <c r="K22" s="69"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="69">
+      <c r="M22" s="71"/>
+      <c r="N22" s="70">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="67"/>
+      <c r="P22" s="69"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="69">
+      <c r="R22" s="71"/>
+      <c r="S22" s="70">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="67"/>
+      <c r="U22" s="69"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="68"/>
-      <c r="X22" s="69">
+      <c r="W22" s="71"/>
+      <c r="X22" s="70">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
@@ -1680,74 +1680,74 @@
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="71"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="70" t="s">
+      <c r="D23" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="69"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="67"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="69"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="69"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="70"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="67"/>
+      <c r="P23" s="69"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="69"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="70"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="67"/>
+      <c r="U23" s="69"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="68"/>
-      <c r="X23" s="69"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="67" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="70"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="69">
+      <c r="I24" s="71"/>
+      <c r="J24" s="70">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="67"/>
+      <c r="K24" s="69"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="69">
+      <c r="M24" s="71"/>
+      <c r="N24" s="70">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="67"/>
+      <c r="P24" s="69"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="68"/>
-      <c r="S24" s="69">
+      <c r="R24" s="71"/>
+      <c r="S24" s="70">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="67"/>
+      <c r="U24" s="69"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="68"/>
-      <c r="X24" s="69">
+      <c r="W24" s="71"/>
+      <c r="X24" s="70">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="71"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,24 +1765,24 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="67"/>
+      <c r="G25" s="69"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="67"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="69"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="69"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="70"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="67"/>
+      <c r="P25" s="69"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="69"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="70"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="67"/>
+      <c r="U25" s="69"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="68"/>
-      <c r="X25" s="69"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
@@ -1957,7 +1957,7 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="70" t="s">
+      <c r="D30" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="24"/>
@@ -1991,7 +1991,7 @@
       <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="70"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2210,7 +2210,7 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="70" t="s">
+      <c r="D37" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="24"/>
@@ -2244,7 +2244,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="70"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2411,6 +2411,80 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2426,80 +2500,6 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#105414 Removed two capping cells that were incorrectly included from the original mockup
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37413A0-4C99-4462-AAA8-238AAFAC15D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1404C5-3797-429C-9683-6B025AAEDE79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
@@ -519,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1111,7 +1111,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="31"/>
@@ -1146,41 +1146,41 @@
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="70">
+      <c r="I9" s="68"/>
+      <c r="J9" s="69">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="69"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="71"/>
-      <c r="N9" s="70">
+      <c r="M9" s="68"/>
+      <c r="N9" s="69">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="69"/>
+      <c r="P9" s="67"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="70">
+      <c r="R9" s="68"/>
+      <c r="S9" s="69">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="69"/>
+      <c r="U9" s="67"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="70">
+      <c r="W9" s="68"/>
+      <c r="X9" s="69">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
@@ -1189,72 +1189,72 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="67"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="70"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="69"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="69"/>
+      <c r="P10" s="67"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="70"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="69"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="69"/>
+      <c r="U10" s="67"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="70"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="70">
+      <c r="I11" s="68"/>
+      <c r="J11" s="69">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="69"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="70">
+      <c r="M11" s="68"/>
+      <c r="N11" s="69">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="69"/>
+      <c r="P11" s="67"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="70">
+      <c r="R11" s="68"/>
+      <c r="S11" s="69">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="69"/>
+      <c r="U11" s="67"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="70">
+      <c r="W11" s="68"/>
+      <c r="X11" s="69">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
@@ -1263,74 +1263,74 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="69"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="69"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="70"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="69"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="70"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="69"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="69"/>
+      <c r="U12" s="67"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="70"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="69"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="70">
+      <c r="I13" s="68"/>
+      <c r="J13" s="69">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="69"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="70">
+      <c r="M13" s="68"/>
+      <c r="N13" s="69">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="69"/>
+      <c r="P13" s="67"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="70">
+      <c r="R13" s="68"/>
+      <c r="S13" s="69">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="69"/>
+      <c r="U13" s="67"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="71"/>
-      <c r="X13" s="70">
+      <c r="W13" s="68"/>
+      <c r="X13" s="69">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="67"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1347,25 +1347,25 @@
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="69"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="70"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="69"/>
+      <c r="P14" s="67"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="70"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="69"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="69"/>
+      <c r="U14" s="67"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="71"/>
-      <c r="X14" s="70"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="69"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -1528,7 +1528,7 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="41"/>
@@ -1563,41 +1563,41 @@
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="70"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="69"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="70">
+      <c r="I20" s="68"/>
+      <c r="J20" s="69">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="69"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="70">
+      <c r="M20" s="68"/>
+      <c r="N20" s="69">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="69"/>
+      <c r="P20" s="67"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="71"/>
-      <c r="S20" s="70">
+      <c r="R20" s="68"/>
+      <c r="S20" s="69">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="69"/>
+      <c r="U20" s="67"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="71"/>
-      <c r="X20" s="70">
+      <c r="W20" s="68"/>
+      <c r="X20" s="69">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
@@ -1606,72 +1606,72 @@
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="70" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="69"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="69"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="67"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="70"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="69"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="70"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="69"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="69"/>
+      <c r="U21" s="67"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="70"/>
+      <c r="W21" s="68"/>
+      <c r="X21" s="69"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="72"/>
+      <c r="D22" s="70"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="69"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="70">
+      <c r="I22" s="68"/>
+      <c r="J22" s="69">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="69"/>
+      <c r="K22" s="67"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="70">
+      <c r="M22" s="68"/>
+      <c r="N22" s="69">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="69"/>
+      <c r="P22" s="67"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="70">
+      <c r="R22" s="68"/>
+      <c r="S22" s="69">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="69"/>
+      <c r="U22" s="67"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="71"/>
-      <c r="X22" s="70">
+      <c r="W22" s="68"/>
+      <c r="X22" s="69">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
@@ -1680,74 +1680,74 @@
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="69"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="69"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="67"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="70"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="69"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="69"/>
+      <c r="P23" s="67"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="70"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="69"/>
+      <c r="U23" s="67"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="71"/>
-      <c r="X23" s="70"/>
+      <c r="W23" s="68"/>
+      <c r="X23" s="69"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="72"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="69"/>
+      <c r="G24" s="67"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="70">
+      <c r="I24" s="68"/>
+      <c r="J24" s="69">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="69"/>
+      <c r="K24" s="67"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="70">
+      <c r="M24" s="68"/>
+      <c r="N24" s="69">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="69"/>
+      <c r="P24" s="67"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="70">
+      <c r="R24" s="68"/>
+      <c r="S24" s="69">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="69"/>
+      <c r="U24" s="67"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="70">
+      <c r="W24" s="68"/>
+      <c r="X24" s="69">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,24 +1765,24 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="69"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="69"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="67"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="70"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="69"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="69"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="70"/>
+      <c r="R25" s="68"/>
+      <c r="S25" s="69"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="69"/>
+      <c r="U25" s="67"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="71"/>
-      <c r="X25" s="70"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="69"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
@@ -1957,7 +1957,7 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="24"/>
@@ -1991,7 +1991,7 @@
       <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="72"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2210,7 +2210,7 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="72" t="s">
+      <c r="D37" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="24"/>
@@ -2244,7 +2244,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="72"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2343,10 +2343,7 @@
         <f>SUM(Q40-M40)</f>
         <v>0</v>
       </c>
-      <c r="S40" s="37">
-        <f>SUM(S32:S39)</f>
-        <v>0</v>
-      </c>
+      <c r="S40" s="37"/>
       <c r="T40" s="54"/>
       <c r="U40" s="63"/>
       <c r="V40" s="18">
@@ -2392,10 +2389,7 @@
         <f>R40</f>
         <v>0</v>
       </c>
-      <c r="S41" s="38">
-        <f>SUM(R40:S40)</f>
-        <v>0</v>
-      </c>
+      <c r="S41" s="38"/>
       <c r="T41" s="19"/>
       <c r="U41" s="19"/>
       <c r="V41" s="19"/>
@@ -2411,80 +2405,6 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2500,6 +2420,80 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#105473 #105450 Updating report template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1404C5-3797-429C-9683-6B025AAEDE79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5620D191-5E97-40CB-AD54-8A5BA1030193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
@@ -519,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -854,7 +854,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
@@ -1111,7 +1111,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="72" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="31"/>
@@ -1146,41 +1146,41 @@
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="67" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="67"/>
+      <c r="D9" s="72"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="69">
+      <c r="I9" s="71"/>
+      <c r="J9" s="70">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="67"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="69">
+      <c r="M9" s="71"/>
+      <c r="N9" s="70">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="67"/>
+      <c r="P9" s="69"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="69">
+      <c r="R9" s="71"/>
+      <c r="S9" s="70">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="67"/>
+      <c r="U9" s="69"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="68"/>
-      <c r="X9" s="69">
+      <c r="W9" s="71"/>
+      <c r="X9" s="70">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
@@ -1189,72 +1189,72 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="67"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="69"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="67"/>
+      <c r="P10" s="69"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="69"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="70"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="67"/>
+      <c r="U10" s="69"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="68"/>
-      <c r="X10" s="69"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="70"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="67" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="67"/>
+      <c r="D11" s="72"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69">
+      <c r="I11" s="71"/>
+      <c r="J11" s="70">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="69">
+      <c r="M11" s="71"/>
+      <c r="N11" s="70">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="67"/>
+      <c r="P11" s="69"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="69">
+      <c r="R11" s="71"/>
+      <c r="S11" s="70">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="67"/>
+      <c r="U11" s="69"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="69">
+      <c r="W11" s="71"/>
+      <c r="X11" s="70">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
@@ -1263,74 +1263,74 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="71"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="67"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="69"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="69"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="70"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="67"/>
+      <c r="P12" s="69"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="70"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="67"/>
+      <c r="U12" s="69"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="69"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="70"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="67" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="70"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="69">
+      <c r="I13" s="71"/>
+      <c r="J13" s="70">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="67"/>
+      <c r="K13" s="69"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="69">
+      <c r="M13" s="71"/>
+      <c r="N13" s="70">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="67"/>
+      <c r="P13" s="69"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69">
+      <c r="R13" s="71"/>
+      <c r="S13" s="70">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="67"/>
+      <c r="U13" s="69"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="68"/>
-      <c r="X13" s="69">
+      <c r="W13" s="71"/>
+      <c r="X13" s="70">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1347,25 +1347,25 @@
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="67"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="69"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="69"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="70"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="67"/>
+      <c r="P14" s="69"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="70"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="67"/>
+      <c r="U14" s="69"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="69"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="70"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -1528,7 +1528,7 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="72" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="41"/>
@@ -1563,41 +1563,41 @@
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="67" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="70"/>
+      <c r="D20" s="72"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="67"/>
+      <c r="G20" s="69"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="69">
+      <c r="I20" s="71"/>
+      <c r="J20" s="70">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="67"/>
+      <c r="K20" s="69"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="69">
+      <c r="M20" s="71"/>
+      <c r="N20" s="70">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="67"/>
+      <c r="P20" s="69"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="69">
+      <c r="R20" s="71"/>
+      <c r="S20" s="70">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="67"/>
+      <c r="U20" s="69"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="68"/>
-      <c r="X20" s="69">
+      <c r="W20" s="71"/>
+      <c r="X20" s="70">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
@@ -1606,72 +1606,72 @@
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D21" s="72" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="67"/>
+      <c r="G21" s="69"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="67"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="69"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="69"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="70"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="67"/>
+      <c r="P21" s="69"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="69"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="70"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="67"/>
+      <c r="U21" s="69"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="68"/>
-      <c r="X21" s="69"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="70"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="67" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="70"/>
+      <c r="D22" s="72"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="67"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="69">
+      <c r="I22" s="71"/>
+      <c r="J22" s="70">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="67"/>
+      <c r="K22" s="69"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="69">
+      <c r="M22" s="71"/>
+      <c r="N22" s="70">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="67"/>
+      <c r="P22" s="69"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="69">
+      <c r="R22" s="71"/>
+      <c r="S22" s="70">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="67"/>
+      <c r="U22" s="69"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="68"/>
-      <c r="X22" s="69">
+      <c r="W22" s="71"/>
+      <c r="X22" s="70">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
@@ -1680,74 +1680,74 @@
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="71"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="70" t="s">
+      <c r="D23" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="69"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="67"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="69"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="69"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="70"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="67"/>
+      <c r="P23" s="69"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="69"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="70"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="67"/>
+      <c r="U23" s="69"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="68"/>
-      <c r="X23" s="69"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="67" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="70"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="69">
+      <c r="I24" s="71"/>
+      <c r="J24" s="70">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="67"/>
+      <c r="K24" s="69"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="69">
+      <c r="M24" s="71"/>
+      <c r="N24" s="70">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="67"/>
+      <c r="P24" s="69"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="68"/>
-      <c r="S24" s="69">
+      <c r="R24" s="71"/>
+      <c r="S24" s="70">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="67"/>
+      <c r="U24" s="69"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="68"/>
-      <c r="X24" s="69">
+      <c r="W24" s="71"/>
+      <c r="X24" s="70">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="71"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,24 +1765,24 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="67"/>
+      <c r="G25" s="69"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="67"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="69"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="69"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="70"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="67"/>
+      <c r="P25" s="69"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="69"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="70"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="67"/>
+      <c r="U25" s="69"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="68"/>
-      <c r="X25" s="69"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
@@ -1957,7 +1957,7 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="70" t="s">
+      <c r="D30" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="24"/>
@@ -1991,7 +1991,7 @@
       <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="70"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2210,7 +2210,7 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="70" t="s">
+      <c r="D37" s="72" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="24"/>
@@ -2244,7 +2244,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="70"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2325,7 +2325,7 @@
       <c r="J40" s="37"/>
       <c r="K40" s="63"/>
       <c r="L40" s="18">
-        <f>SUM(L34:L39)</f>
+        <f>SUM(L37:L39)</f>
         <v>0</v>
       </c>
       <c r="M40" s="18">
@@ -2336,11 +2336,11 @@
       <c r="O40" s="54"/>
       <c r="P40" s="63"/>
       <c r="Q40" s="18">
-        <f>SUM(Q34:Q39)</f>
+        <f>SUM(Q37:Q39)</f>
         <v>0</v>
       </c>
       <c r="R40" s="18">
-        <f>SUM(Q40-M40)</f>
+        <f>SUM(Q40-L40)</f>
         <v>0</v>
       </c>
       <c r="S40" s="37"/>
@@ -2405,6 +2405,80 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2420,80 +2494,6 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#105450 Update to template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5620D191-5E97-40CB-AD54-8A5BA1030193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF56323-11B6-410C-ADD5-6A4EBF7FE863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
@@ -519,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -854,7 +854,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
@@ -1111,7 +1111,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="31"/>
@@ -1146,41 +1146,41 @@
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="70">
+      <c r="I9" s="68"/>
+      <c r="J9" s="69">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="69"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="71"/>
-      <c r="N9" s="70">
+      <c r="M9" s="68"/>
+      <c r="N9" s="69">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="69"/>
+      <c r="P9" s="67"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="70">
+      <c r="R9" s="68"/>
+      <c r="S9" s="69">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="69"/>
+      <c r="U9" s="67"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="70">
+      <c r="W9" s="68"/>
+      <c r="X9" s="69">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
@@ -1189,72 +1189,72 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="67"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="70"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="69"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="69"/>
+      <c r="P10" s="67"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="70"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="69"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="69"/>
+      <c r="U10" s="67"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="70"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="70">
+      <c r="I11" s="68"/>
+      <c r="J11" s="69">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="69"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="70">
+      <c r="M11" s="68"/>
+      <c r="N11" s="69">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="69"/>
+      <c r="P11" s="67"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="70">
+      <c r="R11" s="68"/>
+      <c r="S11" s="69">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="69"/>
+      <c r="U11" s="67"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="70">
+      <c r="W11" s="68"/>
+      <c r="X11" s="69">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
@@ -1263,74 +1263,74 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="69"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="69"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="70"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="69"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="70"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="69"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="69"/>
+      <c r="U12" s="67"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="70"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="69"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="70">
+      <c r="I13" s="68"/>
+      <c r="J13" s="69">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="69"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="70">
+      <c r="M13" s="68"/>
+      <c r="N13" s="69">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="69"/>
+      <c r="P13" s="67"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="70">
+      <c r="R13" s="68"/>
+      <c r="S13" s="69">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="69"/>
+      <c r="U13" s="67"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="71"/>
-      <c r="X13" s="70">
+      <c r="W13" s="68"/>
+      <c r="X13" s="69">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="67"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1347,25 +1347,25 @@
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="69"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="70"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="69"/>
+      <c r="P14" s="67"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="70"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="69"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="69"/>
+      <c r="U14" s="67"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="71"/>
-      <c r="X14" s="70"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="69"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -1528,7 +1528,7 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="41"/>
@@ -1563,41 +1563,41 @@
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="70"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="69"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="70">
+      <c r="I20" s="68"/>
+      <c r="J20" s="69">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="69"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="70">
+      <c r="M20" s="68"/>
+      <c r="N20" s="69">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="69"/>
+      <c r="P20" s="67"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="71"/>
-      <c r="S20" s="70">
+      <c r="R20" s="68"/>
+      <c r="S20" s="69">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="69"/>
+      <c r="U20" s="67"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="71"/>
-      <c r="X20" s="70">
+      <c r="W20" s="68"/>
+      <c r="X20" s="69">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
@@ -1606,72 +1606,72 @@
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="70" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="69"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="69"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="67"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="70"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="69"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="70"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="69"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="69"/>
+      <c r="U21" s="67"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="70"/>
+      <c r="W21" s="68"/>
+      <c r="X21" s="69"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="72"/>
+      <c r="D22" s="70"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="69"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="70">
+      <c r="I22" s="68"/>
+      <c r="J22" s="69">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="69"/>
+      <c r="K22" s="67"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="70">
+      <c r="M22" s="68"/>
+      <c r="N22" s="69">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="69"/>
+      <c r="P22" s="67"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="70">
+      <c r="R22" s="68"/>
+      <c r="S22" s="69">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="69"/>
+      <c r="U22" s="67"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="71"/>
-      <c r="X22" s="70">
+      <c r="W22" s="68"/>
+      <c r="X22" s="69">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
@@ -1680,74 +1680,74 @@
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="67"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="69"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="69"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="67"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="70"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="69"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="69"/>
+      <c r="P23" s="67"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="70"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="69"/>
+      <c r="U23" s="67"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="71"/>
-      <c r="X23" s="70"/>
+      <c r="W23" s="68"/>
+      <c r="X23" s="69"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="71" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="72"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="69"/>
+      <c r="G24" s="67"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="70">
+      <c r="I24" s="68"/>
+      <c r="J24" s="69">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="69"/>
+      <c r="K24" s="67"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="70">
+      <c r="M24" s="68"/>
+      <c r="N24" s="69">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="69"/>
+      <c r="P24" s="67"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="70">
+      <c r="R24" s="68"/>
+      <c r="S24" s="69">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="69"/>
+      <c r="U24" s="67"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="70">
+      <c r="W24" s="68"/>
+      <c r="X24" s="69">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="67"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1765,24 +1765,24 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="69"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="69"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="67"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="70"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="69"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="69"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="70"/>
+      <c r="R25" s="68"/>
+      <c r="S25" s="69"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="69"/>
+      <c r="U25" s="67"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="71"/>
-      <c r="X25" s="70"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="69"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
@@ -1957,7 +1957,7 @@
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="24"/>
@@ -1991,7 +1991,7 @@
       <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="72"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2070,7 +2070,7 @@
       <c r="J33" s="37"/>
       <c r="K33" s="63"/>
       <c r="L33" s="18">
-        <f>SUM(L27:L32)</f>
+        <f>SUM(L30:L32)</f>
         <v>0</v>
       </c>
       <c r="M33" s="18">
@@ -2081,7 +2081,7 @@
       <c r="O33" s="54"/>
       <c r="P33" s="63"/>
       <c r="Q33" s="18">
-        <f>SUM(Q27:Q32)</f>
+        <f>SUM(Q30:Q32)</f>
         <v>0</v>
       </c>
       <c r="R33" s="18">
@@ -2092,7 +2092,7 @@
       <c r="T33" s="54"/>
       <c r="U33" s="63"/>
       <c r="V33" s="18">
-        <f>SUM(V27:V32)</f>
+        <f>SUM(V30:V32)</f>
         <v>0</v>
       </c>
       <c r="W33" s="18">
@@ -2210,7 +2210,7 @@
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="72" t="s">
+      <c r="D37" s="70" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="24"/>
@@ -2244,7 +2244,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="72"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2347,7 +2347,7 @@
       <c r="T40" s="54"/>
       <c r="U40" s="63"/>
       <c r="V40" s="18">
-        <f>SUM(V34:V39)</f>
+        <f>SUM(V37:V39)</f>
         <v>0</v>
       </c>
       <c r="W40" s="18">
@@ -2405,80 +2405,6 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2494,6 +2420,80 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#105732 Cross Year report changes
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF56323-11B6-410C-ADD5-6A4EBF7FE863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA58A4B-183E-428A-95D0-F6BC93967685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
-  <si>
-    <t>YNLP-1630</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>FSR Period</t>
   </si>
@@ -66,9 +63,6 @@
     <t>Aug 2020 - Mar 2021</t>
   </si>
   <si>
-    <t>ANLP-1644</t>
-  </si>
-  <si>
     <t>R12 Reconciliation</t>
   </si>
   <si>
@@ -90,12 +84,6 @@
     <t>2020/21</t>
   </si>
   <si>
-    <t>NLA-5899;NLA-1359</t>
-  </si>
-  <si>
-    <t>LEVY-5899;LEVY-2117</t>
-  </si>
-  <si>
     <t>R01 Reconciliation</t>
   </si>
   <si>
@@ -141,15 +129,9 @@
     <t>Sub-total</t>
   </si>
   <si>
-    <t>Indicative payment (reconciliation - capping)</t>
-  </si>
-  <si>
     <t>Payments up to R11</t>
   </si>
   <si>
-    <t>R14 FSR value from previous years</t>
-  </si>
-  <si>
     <t xml:space="preserve">FSR value at R12 </t>
   </si>
   <si>
@@ -196,6 +178,18 @@
   </si>
   <si>
     <t>Contract value at R03</t>
+  </si>
+  <si>
+    <t>FSR value from previous years</t>
+  </si>
+  <si>
+    <t>Indicative payment (reconciliation minus capping)</t>
+  </si>
+  <si>
+    <t>Aug 2018 - Jul 2019</t>
+  </si>
+  <si>
+    <t>R13 and R14 only</t>
   </si>
 </sst>
 </file>
@@ -205,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +256,12 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,22 +519,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -851,7 +851,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214C4B30-7B6D-4E3D-B5EE-3C9FE23BFB4C}">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
@@ -892,7 +892,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4"/>
       <c r="D1" s="14"/>
@@ -910,32 +910,32 @@
     </row>
     <row r="2" spans="1:25" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4"/>
       <c r="D2" s="14"/>
       <c r="F2" s="27"/>
       <c r="G2" s="56" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
       <c r="J2" s="35"/>
       <c r="K2" s="56" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L2" s="57"/>
       <c r="M2" s="57"/>
       <c r="N2" s="35"/>
       <c r="O2" s="56" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="P2" s="58"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="35"/>
       <c r="T2" s="56" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="U2" s="58"/>
       <c r="V2" s="57"/>
@@ -944,10 +944,10 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" s="14"/>
       <c r="F3" s="27"/>
@@ -976,76 +976,76 @@
     </row>
     <row r="5" spans="1:25" s="43" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="X5" s="28" t="s">
         <v>24</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5" s="28" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
     </row>
     <row r="7" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1102,17 +1102,14 @@
       <c r="Y7" s="60"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="70" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="31"/>
       <c r="H8" s="21"/>
@@ -1143,236 +1140,216 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="72"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="70">
+        <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="69"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="70">
+        <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="70">
+        <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="21"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="70">
+        <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B10" s="67"/>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="70"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B11" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="70">
+        <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="69"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="70">
+        <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="21"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="70">
+        <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="21"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="70">
+        <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B12" s="67"/>
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="70"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="69">
-        <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="67"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="69">
-        <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="69">
-        <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="21"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="68"/>
-      <c r="X9" s="69">
-        <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="70" t="s">
+      <c r="D12" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="70"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="70"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B13" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="70">
+        <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="69"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="70">
+        <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="61"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="71"/>
+      <c r="S13" s="70">
+        <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="61"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="71"/>
+      <c r="X13" s="70">
+        <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B14" s="67"/>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="68"/>
-      <c r="X10" s="69"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="70"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69">
-        <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="67"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="69">
-        <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="69">
-        <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T11" s="21"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="69">
-        <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="69"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="69">
-        <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="67"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="69">
-        <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="61"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69">
-        <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="61"/>
-      <c r="U13" s="67"/>
-      <c r="V13" s="61"/>
-      <c r="W13" s="68"/>
-      <c r="X13" s="69">
-        <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>20</v>
-      </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="67"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="69"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="69"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="70"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="67"/>
+      <c r="P14" s="69"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="70"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="67"/>
+      <c r="U14" s="69"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="69"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="70"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>0</v>
-      </c>
+      <c r="A15" s="32"/>
       <c r="B15" s="33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="15"/>
@@ -1435,11 +1412,9 @@
       <c r="Y15" s="64"/>
     </row>
     <row r="16" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="A16" s="5"/>
       <c r="B16" s="11" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="16"/>
@@ -1491,7 +1466,7 @@
     </row>
     <row r="18" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1519,17 +1494,14 @@
       <c r="Y18" s="60"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="70" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>15</v>
       </c>
       <c r="F19" s="41"/>
       <c r="H19" s="21"/>
@@ -1560,236 +1532,216 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="72"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="70">
+        <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="69"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="70">
+        <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="21"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="70">
+        <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="21"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="71"/>
+      <c r="X20" s="70">
+        <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B21" s="67"/>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="69"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="70"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B22" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="70">
+        <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="69"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="70">
+        <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="21"/>
+      <c r="P22" s="69"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="70">
+        <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="21"/>
+      <c r="U22" s="69"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="71"/>
+      <c r="X22" s="70">
+        <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B23" s="67"/>
+      <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="70"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="69">
-        <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="67"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="69">
-        <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O20" s="21"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="69">
-        <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T20" s="21"/>
-      <c r="U20" s="67"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="68"/>
-      <c r="X20" s="69">
-        <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="67"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="68"/>
-      <c r="X21" s="69"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="70"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="69">
-        <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="67"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="69">
-        <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="69">
-        <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="21"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="68"/>
-      <c r="X22" s="69">
-        <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="70" t="s">
-        <v>19</v>
+      <c r="D23" s="72" t="s">
+        <v>17</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="69"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="67"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="69"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="69"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="70"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="67"/>
+      <c r="P23" s="69"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="69"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="70"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="67"/>
+      <c r="U23" s="69"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="68"/>
-      <c r="X23" s="69"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="71" t="s">
-        <v>11</v>
+      <c r="B24" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="70"/>
+        <v>3</v>
+      </c>
+      <c r="D24" s="72"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="69">
+      <c r="I24" s="71"/>
+      <c r="J24" s="70">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="67"/>
+      <c r="K24" s="69"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="69">
+      <c r="M24" s="71"/>
+      <c r="N24" s="70">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="67"/>
+      <c r="P24" s="69"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="68"/>
-      <c r="S24" s="69">
+      <c r="R24" s="71"/>
+      <c r="S24" s="70">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="67"/>
+      <c r="U24" s="69"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="68"/>
-      <c r="X24" s="69">
+      <c r="W24" s="71"/>
+      <c r="X24" s="70">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="71"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="67"/>
+      <c r="G25" s="69"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="67"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="69"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="69"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="70"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="67"/>
+      <c r="P25" s="69"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="69"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="70"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="67"/>
+      <c r="U25" s="69"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="68"/>
-      <c r="X25" s="69"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="A26" s="32"/>
       <c r="B26" s="33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="15"/>
@@ -1852,11 +1804,9 @@
       <c r="Y26" s="64"/>
     </row>
     <row r="27" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="5"/>
       <c r="B27" s="11" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="16"/>
@@ -1920,7 +1870,7 @@
     </row>
     <row r="29" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1948,50 +1898,46 @@
       <c r="Y29" s="60"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="B30" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="24"/>
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30"/>
       <c r="F30" s="31"/>
       <c r="G30" s="24"/>
-      <c r="H30" s="21"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="24"/>
       <c r="J30" s="39"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="21"/>
+      <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="39"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="24"/>
       <c r="P30" s="24"/>
-      <c r="Q30" s="21"/>
+      <c r="Q30" s="24"/>
       <c r="R30" s="24"/>
       <c r="S30" s="39"/>
-      <c r="T30" s="21"/>
+      <c r="T30" s="24"/>
       <c r="U30" s="24"/>
-      <c r="V30" s="21"/>
+      <c r="V30" s="24"/>
       <c r="W30" s="24"/>
       <c r="X30" s="39"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="70"/>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="72" t="s">
+        <v>17</v>
+      </c>
       <c r="E31" s="24"/>
       <c r="F31" s="31"/>
       <c r="G31" s="24"/>
@@ -2014,237 +1960,227 @@
       <c r="X31" s="39"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="B32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="72"/>
       <c r="E32" s="24"/>
       <c r="F32" s="31"/>
       <c r="G32" s="24"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="39"/>
       <c r="K32" s="24"/>
       <c r="L32" s="21"/>
       <c r="M32" s="24"/>
       <c r="N32" s="39"/>
-      <c r="O32" s="62"/>
+      <c r="O32" s="21"/>
       <c r="P32" s="24"/>
       <c r="Q32" s="21"/>
       <c r="R32" s="24"/>
       <c r="S32" s="39"/>
-      <c r="T32" s="62"/>
+      <c r="T32" s="21"/>
       <c r="U32" s="24"/>
       <c r="V32" s="21"/>
       <c r="W32" s="24"/>
       <c r="X32" s="39"/>
     </row>
-    <row r="33" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="26">
-        <f>SUM(H30:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="18">
-        <f>SUM(H33-F33)</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="37"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="18">
-        <f>SUM(L30:L32)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="18">
-        <f>SUM(L33-H33)</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="37"/>
-      <c r="O33" s="54"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="18">
-        <f>SUM(Q30:Q32)</f>
-        <v>0</v>
-      </c>
-      <c r="R33" s="18">
-        <f>SUM(Q33-L33)</f>
-        <v>0</v>
-      </c>
-      <c r="S33" s="37"/>
-      <c r="T33" s="54"/>
-      <c r="U33" s="63"/>
-      <c r="V33" s="18">
-        <f>SUM(V30:V32)</f>
-        <v>0</v>
-      </c>
-      <c r="W33" s="18">
-        <f>SUM(V33-Q33)</f>
-        <v>0</v>
-      </c>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="64"/>
-    </row>
-    <row r="34" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19">
-        <f>I33</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="40"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19">
-        <f>M33</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="40"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19">
-        <f>R33</f>
-        <v>0</v>
-      </c>
-      <c r="S34" s="38"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19">
-        <f>W33</f>
-        <v>0</v>
-      </c>
-      <c r="X34" s="38"/>
-      <c r="Y34" s="65"/>
-    </row>
-    <row r="35" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
-      <c r="B35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="64"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="64"/>
-      <c r="U35" s="66"/>
-      <c r="V35" s="64"/>
-      <c r="W35" s="66"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="64"/>
-    </row>
-    <row r="36" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="53"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="53"/>
-      <c r="W36" s="53"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="60"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="62"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="24"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="62"/>
-      <c r="X37" s="39"/>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="62"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="39"/>
+    </row>
+    <row r="34" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32"/>
+      <c r="B34" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="25">
+        <f>SUM(E30:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="37"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="26">
+        <f>SUM(H31:H33)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="18">
+        <f>(H34-(F34-E34))</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="37"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="18">
+        <f>SUM(L31:L33)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="18">
+        <f>SUM(L34-H34)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="37"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="18">
+        <f>SUM(Q31:Q33)</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="18">
+        <f>SUM(Q34-L34)</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="37"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="63"/>
+      <c r="V34" s="18">
+        <f>SUM(V31:V33)</f>
+        <v>0</v>
+      </c>
+      <c r="W34" s="18">
+        <f>SUM(V34-Q34)</f>
+        <v>0</v>
+      </c>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="64"/>
+    </row>
+    <row r="35" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A35" s="5"/>
+      <c r="B35" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19">
+        <f>I34</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="40"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19">
+        <f>M34</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="40"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19">
+        <f>R34</f>
+        <v>0</v>
+      </c>
+      <c r="S35" s="38"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19">
+        <f>W34</f>
+        <v>0</v>
+      </c>
+      <c r="X35" s="38"/>
+      <c r="Y35" s="65"/>
+    </row>
+    <row r="36" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="45"/>
+      <c r="B36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="64"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="64"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="64"/>
+      <c r="W36" s="66"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="64"/>
+    </row>
+    <row r="37" spans="1:25" s="44" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="53"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
+      <c r="X37" s="30"/>
+      <c r="Y37" s="60"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="70"/>
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="72" t="s">
+        <v>17</v>
+      </c>
       <c r="E38" s="24"/>
       <c r="F38" s="31"/>
       <c r="G38" s="24"/>
@@ -2267,144 +2203,240 @@
       <c r="X38" s="39"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="B39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="72"/>
       <c r="E39" s="24"/>
       <c r="F39" s="31"/>
       <c r="G39" s="24"/>
-      <c r="H39" s="62"/>
+      <c r="H39" s="21"/>
       <c r="I39" s="62"/>
       <c r="J39" s="39"/>
       <c r="K39" s="24"/>
       <c r="L39" s="21"/>
       <c r="M39" s="62"/>
       <c r="N39" s="39"/>
-      <c r="O39" s="62"/>
+      <c r="O39" s="21"/>
       <c r="P39" s="24"/>
       <c r="Q39" s="21"/>
       <c r="R39" s="62"/>
       <c r="S39" s="39"/>
-      <c r="T39" s="62"/>
+      <c r="T39" s="21"/>
       <c r="U39" s="24"/>
       <c r="V39" s="21"/>
       <c r="W39" s="62"/>
       <c r="X39" s="39"/>
     </row>
-    <row r="40" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="37">
-        <v>0</v>
-      </c>
-      <c r="G40" s="63"/>
-      <c r="H40" s="26">
-        <f>SUM(H37:H39)</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="18">
-        <f>SUM(H40-F40)</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="37"/>
-      <c r="K40" s="63"/>
-      <c r="L40" s="18">
-        <f>SUM(L37:L39)</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="18">
-        <f>SUM(L40-H40)</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="37"/>
-      <c r="O40" s="54"/>
-      <c r="P40" s="63"/>
-      <c r="Q40" s="18">
-        <f>SUM(Q37:Q39)</f>
-        <v>0</v>
-      </c>
-      <c r="R40" s="18">
-        <f>SUM(Q40-L40)</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="37"/>
-      <c r="T40" s="54"/>
-      <c r="U40" s="63"/>
-      <c r="V40" s="18">
-        <f>SUM(V37:V39)</f>
-        <v>0</v>
-      </c>
-      <c r="W40" s="18">
-        <f>SUM(V40-Q40)</f>
-        <v>0</v>
-      </c>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="64"/>
-    </row>
-    <row r="41" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19">
-        <f>I40</f>
-        <v>0</v>
-      </c>
-      <c r="J41" s="38"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19">
-        <f>M40</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="38"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19">
-        <f>R40</f>
-        <v>0</v>
-      </c>
-      <c r="S41" s="38"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19">
-        <f>W40</f>
-        <v>0</v>
-      </c>
-      <c r="X41" s="38"/>
-      <c r="Y41" s="65"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A43"/>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="24"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="39"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="62"/>
+      <c r="X40" s="39"/>
+    </row>
+    <row r="41" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="37">
+        <v>0</v>
+      </c>
+      <c r="G41" s="63"/>
+      <c r="H41" s="26">
+        <f>SUM(H38:H40)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="18">
+        <f>SUM(H41-F41)</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="37"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="18">
+        <f>SUM(L38:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="18">
+        <f>SUM(L41-H41)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="37"/>
+      <c r="O41" s="54"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="18">
+        <f>SUM(Q38:Q40)</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="18">
+        <f>SUM(Q41-L41)</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="37"/>
+      <c r="T41" s="54"/>
+      <c r="U41" s="63"/>
+      <c r="V41" s="18">
+        <f>SUM(V38:V40)</f>
+        <v>0</v>
+      </c>
+      <c r="W41" s="18">
+        <f>SUM(V41-Q41)</f>
+        <v>0</v>
+      </c>
+      <c r="X41" s="37"/>
+      <c r="Y41" s="64"/>
+    </row>
+    <row r="42" spans="1:25" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A42" s="5"/>
+      <c r="B42" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19">
+        <f>I41</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="38"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19">
+        <f>M41</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="38"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19">
+        <f>R41</f>
+        <v>0</v>
+      </c>
+      <c r="S42" s="38"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19">
+        <f>W41</f>
+        <v>0</v>
+      </c>
+      <c r="X42" s="38"/>
+      <c r="Y42" s="65"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A44"/>
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2420,81 +2452,8 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
#105732 formatting new column as Currency
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.Reports/Assets/CrossYearPaymentsReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021PEReportService\src\ESFA.DC.PeriodEnd.ReportService.Reports\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA58A4B-183E-428A-95D0-F6BC93967685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697981B6-A54D-4E9D-AB6B-9A2E1E00A995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35C4D588-DEFB-46E4-BD46-53D9271136B1}"/>
   </bookViews>
@@ -323,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -519,24 +519,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,7 +1109,7 @@
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="70" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="31"/>
@@ -1140,185 +1141,185 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="71" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="70">
+      <c r="I9" s="68"/>
+      <c r="J9" s="69">
         <f>IF(SUM(H9:H10)&gt;G9,G9-SUM(H9:H10),0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="69"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="71"/>
-      <c r="N9" s="70">
+      <c r="M9" s="68"/>
+      <c r="N9" s="69">
         <f>IF(SUM(L9:L10)&gt;K9,K9-SUM(L9:L10),0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="69"/>
+      <c r="P9" s="67"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="70">
+      <c r="R9" s="68"/>
+      <c r="S9" s="69">
         <f>IF(SUM(Q9:Q10)&gt;P9,P9-SUM(Q9:Q10),0)</f>
         <v>0</v>
       </c>
       <c r="T9" s="21"/>
-      <c r="U9" s="69"/>
+      <c r="U9" s="67"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="70">
+      <c r="W9" s="68"/>
+      <c r="X9" s="69">
         <f>IF(SUM(V9:V10)&gt;U9,U9-SUM(V9:V10),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B10" s="67"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="67"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="69"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="70"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="69"/>
       <c r="O10" s="21"/>
-      <c r="P10" s="69"/>
+      <c r="P10" s="67"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="70"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="69"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="69"/>
+      <c r="U10" s="67"/>
       <c r="V10" s="21"/>
-      <c r="W10" s="71"/>
-      <c r="X10" s="70"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="69"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="71" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="70">
+      <c r="I11" s="68"/>
+      <c r="J11" s="69">
         <f>IF(SUM(H11:H12)&gt;G11,G11-SUM(H11:H12),0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="69"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="70">
+      <c r="M11" s="68"/>
+      <c r="N11" s="69">
         <f>IF(SUM(L11:L12)&gt;K11,K11-SUM(L11:L12),0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="21"/>
-      <c r="P11" s="69"/>
+      <c r="P11" s="67"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="70">
+      <c r="R11" s="68"/>
+      <c r="S11" s="69">
         <f>IF(SUM(Q11:Q12)&gt;P11,P11-SUM(Q11:Q12),0)</f>
         <v>0</v>
       </c>
       <c r="T11" s="21"/>
-      <c r="U11" s="69"/>
+      <c r="U11" s="67"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="70">
+      <c r="W11" s="68"/>
+      <c r="X11" s="69">
         <f>IF(SUM(V11:V12)&gt;U11,U11-SUM(V11:V12),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B12" s="67"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="70" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="69"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="61"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="69"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="61"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="70"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="61"/>
-      <c r="P12" s="69"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="70"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="69"/>
       <c r="T12" s="61"/>
-      <c r="U12" s="69"/>
+      <c r="U12" s="67"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="70"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="69"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="70">
+      <c r="I13" s="68"/>
+      <c r="J13" s="69">
         <f>IF(SUM(H13:H14)&gt;G13,G13-SUM(H13:H14),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="69"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="70">
+      <c r="M13" s="68"/>
+      <c r="N13" s="69">
         <f>IF(SUM(L13:L14)&gt;K13,K13-SUM(L13:L14),0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="61"/>
-      <c r="P13" s="69"/>
+      <c r="P13" s="67"/>
       <c r="Q13" s="61"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="70">
+      <c r="R13" s="68"/>
+      <c r="S13" s="69">
         <f>IF(SUM(Q13:Q14)&gt;P13,P13-SUM(Q13:Q14),0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="61"/>
-      <c r="U13" s="69"/>
+      <c r="U13" s="67"/>
       <c r="V13" s="61"/>
-      <c r="W13" s="71"/>
-      <c r="X13" s="70">
+      <c r="W13" s="68"/>
+      <c r="X13" s="69">
         <f>IF(SUM(V13:V14)&gt;U13,U13-SUM(V13:V14),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B14" s="67"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1326,25 +1327,25 @@
         <v>18</v>
       </c>
       <c r="E14" s="24"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="67"/>
       <c r="H14" s="62"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="69"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="61"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="70"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="69"/>
+      <c r="P14" s="67"/>
       <c r="Q14" s="61"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="70"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="69"/>
       <c r="T14" s="62"/>
-      <c r="U14" s="69"/>
+      <c r="U14" s="67"/>
       <c r="V14" s="61"/>
-      <c r="W14" s="71"/>
-      <c r="X14" s="70"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="69"/>
     </row>
     <row r="15" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32"/>
@@ -1500,7 +1501,7 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="70" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="41"/>
@@ -1532,185 +1533,185 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="71" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="70"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="69"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="70">
+      <c r="I20" s="68"/>
+      <c r="J20" s="69">
         <f>IF(SUM(H20:H21)&gt;G20,G20-SUM(H20:H21),0)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="69"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="70">
+      <c r="M20" s="68"/>
+      <c r="N20" s="69">
         <f>IF(SUM(L20:L21)&gt;K20,K20-SUM(L20:L21),0)</f>
         <v>0</v>
       </c>
       <c r="O20" s="21"/>
-      <c r="P20" s="69"/>
+      <c r="P20" s="67"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="71"/>
-      <c r="S20" s="70">
+      <c r="R20" s="68"/>
+      <c r="S20" s="69">
         <f>IF(SUM(Q20:Q21)&gt;P20,P20-SUM(Q20:Q21),0)</f>
         <v>0</v>
       </c>
       <c r="T20" s="21"/>
-      <c r="U20" s="69"/>
+      <c r="U20" s="67"/>
       <c r="V20" s="21"/>
-      <c r="W20" s="71"/>
-      <c r="X20" s="70">
+      <c r="W20" s="68"/>
+      <c r="X20" s="69">
         <f>IF(SUM(V20:V21)&gt;U20,U20-SUM(V20:V21),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B21" s="67"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="70" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="41"/>
-      <c r="G21" s="69"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="21"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="69"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="67"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="70"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="69"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="70"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="69"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="69"/>
+      <c r="U21" s="67"/>
       <c r="V21" s="21"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="70"/>
+      <c r="W21" s="68"/>
+      <c r="X21" s="69"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="71" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="72"/>
+      <c r="D22" s="70"/>
       <c r="F22" s="41"/>
-      <c r="G22" s="69"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="21"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="70">
+      <c r="I22" s="68"/>
+      <c r="J22" s="69">
         <f>IF(SUM(H22:H23)&gt;G22,G22-SUM(H22:H23),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="69"/>
+      <c r="K22" s="67"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="70">
+      <c r="M22" s="68"/>
+      <c r="N22" s="69">
         <f>IF(SUM(L22:L23)&gt;K22,K22-SUM(L22:L23),0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="21"/>
-      <c r="P22" s="69"/>
+      <c r="P22" s="67"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="70">
+      <c r="R22" s="68"/>
+      <c r="S22" s="69">
         <f>IF(SUM(Q22:Q23)&gt;P22,P22-SUM(Q22:Q23),0)</f>
         <v>0</v>
       </c>
       <c r="T22" s="21"/>
-      <c r="U22" s="69"/>
+      <c r="U22" s="67"/>
       <c r="V22" s="21"/>
-      <c r="W22" s="71"/>
-      <c r="X22" s="70">
+      <c r="W22" s="68"/>
+      <c r="X22" s="69">
         <f>IF(SUM(V22:V23)&gt;U22,U22-SUM(V22:V23),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B23" s="67"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="70" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="41"/>
-      <c r="G23" s="69"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="61"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="69"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="67"/>
       <c r="L23" s="61"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="70"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="69"/>
       <c r="O23" s="61"/>
-      <c r="P23" s="69"/>
+      <c r="P23" s="67"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="70"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="T23" s="61"/>
-      <c r="U23" s="69"/>
+      <c r="U23" s="67"/>
       <c r="V23" s="61"/>
-      <c r="W23" s="71"/>
-      <c r="X23" s="70"/>
+      <c r="W23" s="68"/>
+      <c r="X23" s="69"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="72"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="24"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="69"/>
+      <c r="G24" s="67"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="70">
+      <c r="I24" s="68"/>
+      <c r="J24" s="69">
         <f>IF(SUM(H24:H25)&gt;G24,G24-SUM(H24:H25),0)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="69"/>
+      <c r="K24" s="67"/>
       <c r="L24" s="61"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="70">
+      <c r="M24" s="68"/>
+      <c r="N24" s="69">
         <f>IF(SUM(L24:L25)&gt;K24,K24-SUM(L24:L25),0)</f>
         <v>0</v>
       </c>
       <c r="O24" s="61"/>
-      <c r="P24" s="69"/>
+      <c r="P24" s="67"/>
       <c r="Q24" s="61"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="70">
+      <c r="R24" s="68"/>
+      <c r="S24" s="69">
         <f>IF(SUM(Q24:Q25)&gt;P24,P24-SUM(Q24:Q25),0)</f>
         <v>0</v>
       </c>
       <c r="T24" s="61"/>
-      <c r="U24" s="69"/>
+      <c r="U24" s="67"/>
       <c r="V24" s="61"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="70">
+      <c r="W24" s="68"/>
+      <c r="X24" s="69">
         <f>IF(SUM(V24:V25)&gt;U24,U24-SUM(V24:V25),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B25" s="67"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1719,24 +1720,24 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="41"/>
-      <c r="G25" s="69"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="62"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="69"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="67"/>
       <c r="L25" s="61"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="70"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="69"/>
       <c r="O25" s="62"/>
-      <c r="P25" s="69"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="61"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="70"/>
+      <c r="R25" s="68"/>
+      <c r="S25" s="69"/>
       <c r="T25" s="62"/>
-      <c r="U25" s="69"/>
+      <c r="U25" s="67"/>
       <c r="V25" s="61"/>
-      <c r="W25" s="71"/>
-      <c r="X25" s="70"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="69"/>
     </row>
     <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32"/>
@@ -1907,7 +1908,7 @@
       <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="E30"/>
+      <c r="E30" s="73"/>
       <c r="F30" s="31"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
@@ -1935,7 +1936,7 @@
       <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="70" t="s">
         <v>17</v>
       </c>
       <c r="E31" s="24"/>
@@ -1966,7 +1967,7 @@
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="72"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="24"/>
       <c r="F32" s="31"/>
       <c r="G32" s="24"/>
@@ -2178,7 +2179,7 @@
       <c r="C38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="70" t="s">
         <v>17</v>
       </c>
       <c r="E38" s="24"/>
@@ -2209,7 +2210,7 @@
       <c r="C39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="72"/>
+      <c r="D39" s="70"/>
       <c r="E39" s="24"/>
       <c r="F39" s="31"/>
       <c r="G39" s="24"/>
@@ -2363,80 +2364,6 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="U22:U23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="U20:U21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -2452,6 +2379,80 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="U20:U21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="U22:U23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>